<commit_message>
demultiplex GB and generalize reaction graph computation
</commit_message>
<xml_diff>
--- a/paper/251021_NF2_library_rechecked_enumerate_v1.xlsx
+++ b/paper/251021_NF2_library_rechecked_enumerate_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adrianomartinelli/projects/delt/delt-core/paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7B772AF-9AD2-624A-B858-2020EF792A57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9615CA0-5AEF-3D40-BEA0-499858952396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4360" yWindow="2240" windowWidth="30240" windowHeight="18880" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" tabRatio="500" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="experiment" sheetId="8" r:id="rId1"/>
@@ -21,7 +21,8 @@
     <sheet name="B1" sheetId="2" r:id="rId6"/>
     <sheet name="compounds" sheetId="3" r:id="rId7"/>
     <sheet name="reactions" sheetId="4" r:id="rId8"/>
-    <sheet name="steps" sheetId="11" r:id="rId9"/>
+    <sheet name="reaction_graph" sheetId="11" r:id="rId9"/>
+    <sheet name="steps" sheetId="12" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="190">
   <si>
     <t>OC(=O)C1=CC(=CN=C1)C#C</t>
   </si>
@@ -358,9 +359,6 @@
     <t>scaffold_6</t>
   </si>
   <si>
-    <t>reactant</t>
-  </si>
-  <si>
     <t>product_1</t>
   </si>
   <si>
@@ -562,9 +560,6 @@
     <t>PASS</t>
   </si>
   <si>
-    <t>experiment-rechecked-enum</t>
-  </si>
-  <si>
     <t>source</t>
   </si>
   <si>
@@ -587,6 +582,39 @@
   </si>
   <si>
     <t>converted_1</t>
+  </si>
+  <si>
+    <t>experiment-rechecked-enum-v1</t>
+  </si>
+  <si>
+    <t>GTCTCACA</t>
+  </si>
+  <si>
+    <t>GTCGTACA</t>
+  </si>
+  <si>
+    <t>GAACCGTA</t>
+  </si>
+  <si>
+    <t>AATCGTTA</t>
+  </si>
+  <si>
+    <t>TGTTGCTA</t>
+  </si>
+  <si>
+    <t>TGGCAATA</t>
+  </si>
+  <si>
+    <t>educt</t>
+  </si>
+  <si>
+    <t>precursor_3</t>
+  </si>
+  <si>
+    <t>educt_2</t>
+  </si>
+  <si>
+    <t>educt_1</t>
   </si>
 </sst>
 </file>
@@ -1415,7 +1443,7 @@
         <v>48</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -1423,7 +1451,7 @@
         <v>58</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -1431,7 +1459,7 @@
         <v>59</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -1444,7 +1472,86 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B7" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{869AAB00-934C-0548-B286-14C9DC635123}">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>187</v>
+      </c>
+      <c r="B3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>172</v>
+      </c>
+      <c r="B6" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>175</v>
+      </c>
+      <c r="B7" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>176</v>
+      </c>
+      <c r="B8" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>104</v>
+      </c>
+      <c r="B9" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>173</v>
+      </c>
+      <c r="B10" t="s">
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -1668,31 +1775,31 @@
         <v>48</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C1" s="21" t="s">
         <v>57</v>
       </c>
       <c r="D1" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>157</v>
+      </c>
+      <c r="F1" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="E1" s="21" t="s">
-        <v>158</v>
-      </c>
-      <c r="F1" s="21" t="s">
+      <c r="G1" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="H1" s="21" t="s">
         <v>154</v>
       </c>
-      <c r="G1" s="21" t="s">
-        <v>161</v>
-      </c>
-      <c r="H1" s="21" t="s">
+      <c r="I1" s="21" t="s">
         <v>155</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="J1" s="21" t="s">
         <v>156</v>
-      </c>
-      <c r="J1" s="21" t="s">
-        <v>157</v>
       </c>
       <c r="K1" s="22" t="s">
         <v>52</v>
@@ -1703,34 +1810,34 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C2" s="26">
         <v>45561</v>
       </c>
       <c r="D2" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>158</v>
+      </c>
+      <c r="F2" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="E2" s="27" t="s">
-        <v>159</v>
-      </c>
-      <c r="F2" s="28" t="s">
+      <c r="G2" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="G2" s="29" t="s">
+      <c r="H2" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="I2" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="I2" s="30" t="s">
+      <c r="J2" s="31" t="s">
         <v>114</v>
-      </c>
-      <c r="J2" s="31" t="s">
-        <v>115</v>
       </c>
       <c r="K2" s="32" t="s">
         <v>69</v>
@@ -1741,34 +1848,34 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="24" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C3" s="26">
         <v>45561</v>
       </c>
       <c r="D3" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="E3" s="27" t="s">
+        <v>158</v>
+      </c>
+      <c r="F3" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="E3" s="27" t="s">
-        <v>159</v>
-      </c>
-      <c r="F3" s="28" t="s">
+      <c r="G3" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="G3" s="29" t="s">
+      <c r="H3" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="H3" s="25" t="s">
+      <c r="I3" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="I3" s="30" t="s">
+      <c r="J3" s="31" t="s">
         <v>114</v>
-      </c>
-      <c r="J3" s="31" t="s">
-        <v>115</v>
       </c>
       <c r="K3" s="32" t="s">
         <v>71</v>
@@ -1779,34 +1886,34 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="24" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C4" s="26">
         <v>45561</v>
       </c>
       <c r="D4" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="E4" s="27" t="s">
+        <v>158</v>
+      </c>
+      <c r="F4" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="E4" s="27" t="s">
-        <v>159</v>
-      </c>
-      <c r="F4" s="28" t="s">
+      <c r="G4" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="G4" s="29" t="s">
+      <c r="H4" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="H4" s="25" t="s">
+      <c r="I4" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="I4" s="30" t="s">
+      <c r="J4" s="31" t="s">
         <v>114</v>
-      </c>
-      <c r="J4" s="31" t="s">
-        <v>115</v>
       </c>
       <c r="K4" s="32" t="s">
         <v>72</v>
@@ -1817,34 +1924,34 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="24" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C5" s="26">
         <v>45561</v>
       </c>
       <c r="D5" s="34" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E5" s="34" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F5" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="G5" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="G5" s="29" t="s">
+      <c r="H5" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="H5" s="25" t="s">
+      <c r="I5" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="I5" s="30" t="s">
+      <c r="J5" s="31" t="s">
         <v>114</v>
-      </c>
-      <c r="J5" s="31" t="s">
-        <v>115</v>
       </c>
       <c r="K5" s="32" t="s">
         <v>12</v>
@@ -1855,34 +1962,34 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="24" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C6" s="26">
         <v>45561</v>
       </c>
       <c r="D6" s="34" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E6" s="34" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F6" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="G6" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="G6" s="29" t="s">
+      <c r="H6" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="H6" s="25" t="s">
+      <c r="I6" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="I6" s="30" t="s">
+      <c r="J6" s="31" t="s">
         <v>114</v>
-      </c>
-      <c r="J6" s="31" t="s">
-        <v>115</v>
       </c>
       <c r="K6" s="32" t="s">
         <v>14</v>
@@ -1893,34 +2000,34 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C7" s="26">
         <v>45561</v>
       </c>
       <c r="D7" s="34" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E7" s="34" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F7" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="G7" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="G7" s="29" t="s">
+      <c r="H7" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="H7" s="25" t="s">
+      <c r="I7" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="I7" s="30" t="s">
+      <c r="J7" s="31" t="s">
         <v>114</v>
-      </c>
-      <c r="J7" s="31" t="s">
-        <v>115</v>
       </c>
       <c r="K7" s="32" t="s">
         <v>73</v>
@@ -1931,34 +2038,34 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="24" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C8" s="26">
         <v>45561</v>
       </c>
       <c r="D8" s="35" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E8" s="35" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F8" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="G8" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="G8" s="29" t="s">
+      <c r="H8" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="H8" s="25" t="s">
+      <c r="I8" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="I8" s="30" t="s">
+      <c r="J8" s="31" t="s">
         <v>114</v>
-      </c>
-      <c r="J8" s="31" t="s">
-        <v>115</v>
       </c>
       <c r="K8" s="32" t="s">
         <v>8</v>
@@ -1969,34 +2076,34 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="24" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C9" s="26">
         <v>45561</v>
       </c>
       <c r="D9" s="35" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E9" s="35" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F9" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="G9" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="G9" s="29" t="s">
+      <c r="H9" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="H9" s="25" t="s">
+      <c r="I9" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="I9" s="30" t="s">
+      <c r="J9" s="31" t="s">
         <v>114</v>
-      </c>
-      <c r="J9" s="31" t="s">
-        <v>115</v>
       </c>
       <c r="K9" s="32" t="s">
         <v>74</v>
@@ -2007,34 +2114,34 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="24" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C10" s="26">
         <v>45561</v>
       </c>
       <c r="D10" s="35" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E10" s="35" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F10" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="G10" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="G10" s="29" t="s">
+      <c r="H10" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="H10" s="25" t="s">
+      <c r="I10" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="I10" s="30" t="s">
+      <c r="J10" s="31" t="s">
         <v>114</v>
-      </c>
-      <c r="J10" s="31" t="s">
-        <v>115</v>
       </c>
       <c r="K10" s="32" t="s">
         <v>75</v>
@@ -2045,34 +2152,34 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C11" s="26">
         <v>45561</v>
       </c>
       <c r="D11" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="E11" s="27" t="s">
+        <v>158</v>
+      </c>
+      <c r="F11" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="E11" s="27" t="s">
-        <v>159</v>
-      </c>
-      <c r="F11" s="28" t="s">
+      <c r="G11" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="G11" s="29" t="s">
+      <c r="H11" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="H11" s="25" t="s">
-        <v>113</v>
-      </c>
       <c r="I11" s="36" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J11" s="31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K11" s="32" t="s">
         <v>76</v>
@@ -2083,34 +2190,34 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="24" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C12" s="26">
         <v>45561</v>
       </c>
       <c r="D12" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="E12" s="27" t="s">
+        <v>158</v>
+      </c>
+      <c r="F12" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="E12" s="27" t="s">
-        <v>159</v>
-      </c>
-      <c r="F12" s="28" t="s">
+      <c r="G12" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="G12" s="29" t="s">
+      <c r="H12" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="H12" s="25" t="s">
-        <v>113</v>
-      </c>
       <c r="I12" s="36" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J12" s="31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K12" s="32" t="s">
         <v>77</v>
@@ -2121,34 +2228,34 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="24" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C13" s="26">
         <v>45561</v>
       </c>
       <c r="D13" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="E13" s="27" t="s">
+        <v>158</v>
+      </c>
+      <c r="F13" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="E13" s="27" t="s">
-        <v>159</v>
-      </c>
-      <c r="F13" s="28" t="s">
+      <c r="G13" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="G13" s="29" t="s">
+      <c r="H13" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="H13" s="25" t="s">
-        <v>113</v>
-      </c>
       <c r="I13" s="36" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J13" s="31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K13" s="32" t="s">
         <v>78</v>
@@ -2159,34 +2266,34 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="24" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C14" s="26">
         <v>45561</v>
       </c>
       <c r="D14" s="37" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E14" s="37" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F14" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="G14" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="G14" s="29" t="s">
+      <c r="H14" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="H14" s="25" t="s">
-        <v>113</v>
-      </c>
       <c r="I14" s="36" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J14" s="31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K14" s="32" t="s">
         <v>79</v>
@@ -2197,34 +2304,34 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="24" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C15" s="26">
         <v>45561</v>
       </c>
       <c r="D15" s="37" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E15" s="37" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F15" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="G15" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="G15" s="29" t="s">
+      <c r="H15" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="H15" s="25" t="s">
-        <v>113</v>
-      </c>
       <c r="I15" s="36" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J15" s="31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K15" s="32" t="s">
         <v>80</v>
@@ -2235,34 +2342,34 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="24" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C16" s="26">
         <v>45561</v>
       </c>
       <c r="D16" s="37" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E16" s="37" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F16" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="G16" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="G16" s="29" t="s">
+      <c r="H16" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="H16" s="25" t="s">
-        <v>113</v>
-      </c>
       <c r="I16" s="36" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J16" s="31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K16" s="32" t="s">
         <v>81</v>
@@ -2273,34 +2380,34 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="24" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C17" s="26">
         <v>45561</v>
       </c>
       <c r="D17" s="38" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E17" s="38" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F17" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="G17" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="G17" s="29" t="s">
+      <c r="H17" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="H17" s="25" t="s">
-        <v>113</v>
-      </c>
       <c r="I17" s="36" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J17" s="31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K17" s="32" t="s">
         <v>82</v>
@@ -2311,34 +2418,34 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B18" s="25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C18" s="26">
         <v>45561</v>
       </c>
       <c r="D18" s="38" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E18" s="38" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F18" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="G18" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="G18" s="29" t="s">
+      <c r="H18" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="H18" s="25" t="s">
-        <v>113</v>
-      </c>
       <c r="I18" s="36" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J18" s="31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K18" s="32" t="s">
         <v>83</v>
@@ -2349,34 +2456,34 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="24" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B19" s="25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C19" s="26">
         <v>45561</v>
       </c>
       <c r="D19" s="38" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E19" s="38" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F19" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="G19" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="G19" s="29" t="s">
+      <c r="H19" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="H19" s="25" t="s">
-        <v>113</v>
-      </c>
       <c r="I19" s="36" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J19" s="31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K19" s="32" t="s">
         <v>84</v>
@@ -2387,34 +2494,34 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="24" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C20" s="26">
         <v>45582</v>
       </c>
       <c r="D20" s="27" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E20" s="27" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F20" s="39" t="s">
+        <v>138</v>
+      </c>
+      <c r="G20" s="29" t="s">
+        <v>111</v>
+      </c>
+      <c r="H20" s="25" t="s">
         <v>139</v>
       </c>
-      <c r="G20" s="29" t="s">
-        <v>112</v>
-      </c>
-      <c r="H20" s="25" t="s">
+      <c r="I20" s="37" t="s">
         <v>140</v>
       </c>
-      <c r="I20" s="37" t="s">
-        <v>141</v>
-      </c>
       <c r="J20" s="31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K20" s="32" t="s">
         <v>85</v>
@@ -2425,34 +2532,34 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="24" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C21" s="26">
         <v>45582</v>
       </c>
       <c r="D21" s="27" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E21" s="27" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F21" s="39" t="s">
+        <v>138</v>
+      </c>
+      <c r="G21" s="29" t="s">
+        <v>111</v>
+      </c>
+      <c r="H21" s="25" t="s">
         <v>139</v>
       </c>
-      <c r="G21" s="29" t="s">
-        <v>112</v>
-      </c>
-      <c r="H21" s="25" t="s">
+      <c r="I21" s="37" t="s">
         <v>140</v>
       </c>
-      <c r="I21" s="37" t="s">
-        <v>141</v>
-      </c>
       <c r="J21" s="31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K21" s="32" t="s">
         <v>86</v>
@@ -2463,34 +2570,34 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="24" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B22" s="25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C22" s="26">
         <v>45582</v>
       </c>
       <c r="D22" s="27" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E22" s="27" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F22" s="39" t="s">
+        <v>138</v>
+      </c>
+      <c r="G22" s="29" t="s">
+        <v>111</v>
+      </c>
+      <c r="H22" s="25" t="s">
         <v>139</v>
       </c>
-      <c r="G22" s="29" t="s">
-        <v>112</v>
-      </c>
-      <c r="H22" s="25" t="s">
+      <c r="I22" s="37" t="s">
         <v>140</v>
       </c>
-      <c r="I22" s="37" t="s">
-        <v>141</v>
-      </c>
       <c r="J22" s="31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K22" s="32" t="s">
         <v>87</v>
@@ -2501,34 +2608,34 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="24" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B23" s="25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C23" s="26">
         <v>45582</v>
       </c>
       <c r="D23" s="40" t="s">
+        <v>144</v>
+      </c>
+      <c r="E23" s="40" t="s">
+        <v>159</v>
+      </c>
+      <c r="F23" s="39" t="s">
+        <v>138</v>
+      </c>
+      <c r="G23" s="30" t="s">
         <v>145</v>
       </c>
-      <c r="E23" s="40" t="s">
-        <v>160</v>
-      </c>
-      <c r="F23" s="39" t="s">
+      <c r="H23" s="25" t="s">
         <v>139</v>
       </c>
-      <c r="G23" s="30" t="s">
-        <v>146</v>
-      </c>
-      <c r="H23" s="25" t="s">
+      <c r="I23" s="37" t="s">
         <v>140</v>
       </c>
-      <c r="I23" s="37" t="s">
-        <v>141</v>
-      </c>
       <c r="J23" s="31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K23" s="32" t="s">
         <v>88</v>
@@ -2539,34 +2646,34 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="24" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B24" s="25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C24" s="26">
         <v>45582</v>
       </c>
       <c r="D24" s="40" t="s">
+        <v>144</v>
+      </c>
+      <c r="E24" s="40" t="s">
+        <v>159</v>
+      </c>
+      <c r="F24" s="39" t="s">
+        <v>138</v>
+      </c>
+      <c r="G24" s="30" t="s">
         <v>145</v>
       </c>
-      <c r="E24" s="40" t="s">
-        <v>160</v>
-      </c>
-      <c r="F24" s="39" t="s">
+      <c r="H24" s="25" t="s">
         <v>139</v>
       </c>
-      <c r="G24" s="30" t="s">
-        <v>146</v>
-      </c>
-      <c r="H24" s="25" t="s">
+      <c r="I24" s="37" t="s">
         <v>140</v>
       </c>
-      <c r="I24" s="37" t="s">
-        <v>141</v>
-      </c>
       <c r="J24" s="31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K24" s="32" t="s">
         <v>15</v>
@@ -2577,34 +2684,34 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="24" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B25" s="25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C25" s="26">
         <v>45582</v>
       </c>
       <c r="D25" s="40" t="s">
+        <v>144</v>
+      </c>
+      <c r="E25" s="40" t="s">
+        <v>159</v>
+      </c>
+      <c r="F25" s="39" t="s">
+        <v>138</v>
+      </c>
+      <c r="G25" s="30" t="s">
         <v>145</v>
       </c>
-      <c r="E25" s="40" t="s">
-        <v>160</v>
-      </c>
-      <c r="F25" s="39" t="s">
+      <c r="H25" s="25" t="s">
         <v>139</v>
       </c>
-      <c r="G25" s="30" t="s">
-        <v>146</v>
-      </c>
-      <c r="H25" s="25" t="s">
+      <c r="I25" s="37" t="s">
         <v>140</v>
       </c>
-      <c r="I25" s="37" t="s">
-        <v>141</v>
-      </c>
       <c r="J25" s="31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K25" s="32" t="s">
         <v>13</v>
@@ -2615,34 +2722,34 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="24" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B26" s="25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C26" s="26">
         <v>45582</v>
       </c>
       <c r="D26" s="40" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E26" s="40" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F26" s="39" t="s">
+        <v>138</v>
+      </c>
+      <c r="G26" s="41" t="s">
+        <v>149</v>
+      </c>
+      <c r="H26" s="25" t="s">
         <v>139</v>
       </c>
-      <c r="G26" s="41" t="s">
-        <v>150</v>
-      </c>
-      <c r="H26" s="25" t="s">
+      <c r="I26" s="37" t="s">
         <v>140</v>
       </c>
-      <c r="I26" s="37" t="s">
-        <v>141</v>
-      </c>
       <c r="J26" s="31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K26" s="32" t="s">
         <v>89</v>
@@ -2653,34 +2760,34 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="24" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B27" s="25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C27" s="26">
         <v>45582</v>
       </c>
       <c r="D27" s="40" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E27" s="40" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F27" s="39" t="s">
+        <v>138</v>
+      </c>
+      <c r="G27" s="41" t="s">
+        <v>149</v>
+      </c>
+      <c r="H27" s="25" t="s">
         <v>139</v>
       </c>
-      <c r="G27" s="41" t="s">
-        <v>150</v>
-      </c>
-      <c r="H27" s="25" t="s">
+      <c r="I27" s="37" t="s">
         <v>140</v>
       </c>
-      <c r="I27" s="37" t="s">
-        <v>141</v>
-      </c>
       <c r="J27" s="31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K27" s="32" t="s">
         <v>90</v>
@@ -2691,34 +2798,34 @@
     </row>
     <row r="28" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="42" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B28" s="43" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C28" s="44">
         <v>45582</v>
       </c>
       <c r="D28" s="45" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E28" s="45" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F28" s="46" t="s">
+        <v>138</v>
+      </c>
+      <c r="G28" s="47" t="s">
+        <v>149</v>
+      </c>
+      <c r="H28" s="43" t="s">
         <v>139</v>
       </c>
-      <c r="G28" s="47" t="s">
-        <v>150</v>
-      </c>
-      <c r="H28" s="43" t="s">
+      <c r="I28" s="48" t="s">
         <v>140</v>
       </c>
-      <c r="I28" s="48" t="s">
-        <v>141</v>
-      </c>
       <c r="J28" s="49" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K28" s="50" t="s">
         <v>91</v>
@@ -4496,8 +4603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J612"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4520,7 +4627,7 @@
         <v>44</v>
       </c>
       <c r="D1" s="53" t="s">
-        <v>104</v>
+        <v>186</v>
       </c>
       <c r="E1" s="54" t="s">
         <v>97</v>
@@ -4541,7 +4648,7 @@
         <v>98</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G2" s="67"/>
       <c r="H2" s="67"/>
@@ -4559,7 +4666,7 @@
         <v>98</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G3" s="67"/>
       <c r="H3" s="67"/>
@@ -4580,7 +4687,7 @@
         <v>101</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G4" s="67"/>
       <c r="H4" s="67"/>
@@ -4598,7 +4705,7 @@
         <v>99</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G5" s="67"/>
       <c r="H5" s="67"/>
@@ -4619,7 +4726,7 @@
         <v>102</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G6" s="67"/>
       <c r="H6" s="67"/>
@@ -4637,10 +4744,10 @@
         <v>30</v>
       </c>
       <c r="D7" s="55" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -7151,7 +7258,7 @@
   <dimension ref="A1:E261"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7174,7 +7281,7 @@
         <v>44</v>
       </c>
       <c r="D1" s="60" t="s">
-        <v>104</v>
+        <v>186</v>
       </c>
       <c r="E1" s="61" t="s">
         <v>97</v>
@@ -7191,10 +7298,10 @@
         <v>18</v>
       </c>
       <c r="D2" s="57" t="s">
+        <v>104</v>
+      </c>
+      <c r="E2" s="57" t="s">
         <v>105</v>
-      </c>
-      <c r="E2" s="57" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -7208,10 +7315,10 @@
         <v>18</v>
       </c>
       <c r="D3" s="57" t="s">
+        <v>104</v>
+      </c>
+      <c r="E3" s="57" t="s">
         <v>105</v>
-      </c>
-      <c r="E3" s="57" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -7225,10 +7332,10 @@
         <v>22</v>
       </c>
       <c r="D4" s="57" t="s">
+        <v>104</v>
+      </c>
+      <c r="E4" s="57" t="s">
         <v>105</v>
-      </c>
-      <c r="E4" s="57" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -7242,10 +7349,10 @@
         <v>22</v>
       </c>
       <c r="D5" s="57" t="s">
+        <v>104</v>
+      </c>
+      <c r="E5" s="57" t="s">
         <v>105</v>
-      </c>
-      <c r="E5" s="57" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -7257,25 +7364,25 @@
         <v>26</v>
       </c>
       <c r="D6" s="57" t="s">
+        <v>104</v>
+      </c>
+      <c r="E6" s="57" t="s">
         <v>105</v>
-      </c>
-      <c r="E6" s="57" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="72"/>
       <c r="B7" s="73" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C7" s="74" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D7" s="57" t="s">
+        <v>104</v>
+      </c>
+      <c r="E7" s="57" t="s">
         <v>105</v>
-      </c>
-      <c r="E7" s="57" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -7283,16 +7390,16 @@
         <v>16</v>
       </c>
       <c r="B8" s="56" t="s">
-        <v>17</v>
+        <v>180</v>
       </c>
       <c r="C8" s="56" t="s">
         <v>18</v>
       </c>
       <c r="D8" s="57" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E8" s="57" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -7300,16 +7407,16 @@
         <v>19</v>
       </c>
       <c r="B9" s="56" t="s">
-        <v>20</v>
+        <v>181</v>
       </c>
       <c r="C9" s="56" t="s">
         <v>18</v>
       </c>
       <c r="D9" s="57" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E9" s="57" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -7317,16 +7424,16 @@
         <v>3</v>
       </c>
       <c r="B10" s="58" t="s">
-        <v>21</v>
+        <v>182</v>
       </c>
       <c r="C10" s="56" t="s">
         <v>22</v>
       </c>
       <c r="D10" s="57" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E10" s="57" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -7334,46 +7441,46 @@
         <v>23</v>
       </c>
       <c r="B11" s="58" t="s">
-        <v>24</v>
+        <v>183</v>
       </c>
       <c r="C11" s="56" t="s">
         <v>22</v>
       </c>
       <c r="D11" s="57" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E11" s="57" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="72"/>
       <c r="B12" s="56" t="s">
-        <v>25</v>
+        <v>184</v>
       </c>
       <c r="C12" s="56" t="s">
         <v>26</v>
       </c>
       <c r="D12" s="57" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E12" s="57" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="72"/>
       <c r="B13" s="73" t="s">
-        <v>169</v>
+        <v>185</v>
       </c>
       <c r="C13" s="74" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D13" s="57" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E13" s="57" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -7753,7 +7860,7 @@
         <v>42</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -7764,7 +7871,7 @@
         <v>27</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -7775,7 +7882,7 @@
         <v>28</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -7786,7 +7893,7 @@
         <v>29</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.2">
@@ -7797,7 +7904,7 @@
         <v>93</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.2">
@@ -7808,7 +7915,7 @@
         <v>95</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -7819,12 +7926,12 @@
         <v>96</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B8" s="71" t="s">
         <v>96</v>
@@ -7880,7 +7987,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -7941,22 +8048,22 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -7967,71 +8074,63 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8331A7E-099A-5C4B-BDD9-5519D2C3E2A2}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C3" t="s">
+        <v>176</v>
+      </c>
+      <c r="D3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C4" t="s">
         <v>173</v>
       </c>
-      <c r="B1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>176</v>
-      </c>
-      <c r="B2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>174</v>
-      </c>
-      <c r="B3" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>177</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>178</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>178</v>
-      </c>
-      <c r="B5" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>105</v>
-      </c>
-      <c r="B6" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>175</v>
-      </c>
-      <c r="B7" t="s">
-        <v>180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>